<commit_message>
correção da taxa de juros
</commit_message>
<xml_diff>
--- a/simulador_carro_com_iof.xlsx
+++ b/simulador_carro_com_iof.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,22 +475,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C2" t="n">
-        <v>1468.43</v>
+        <v>1351.94</v>
       </c>
       <c r="D2" t="n">
-        <v>906.3200000000001</v>
+        <v>946.2</v>
       </c>
       <c r="E2" t="n">
-        <v>89828.24000000001</v>
+        <v>89788.36</v>
       </c>
       <c r="F2" t="n">
-        <v>1468.43</v>
+        <v>1351.94</v>
       </c>
       <c r="G2" t="n">
-        <v>906.3200000000001</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +498,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C3" t="n">
-        <v>1453.76</v>
+        <v>1337.85</v>
       </c>
       <c r="D3" t="n">
-        <v>920.99</v>
+        <v>960.3</v>
       </c>
       <c r="E3" t="n">
-        <v>88907.25</v>
+        <v>88828.07000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>2922.19</v>
+        <v>2689.79</v>
       </c>
       <c r="G3" t="n">
-        <v>1827.31</v>
+        <v>1906.5</v>
       </c>
     </row>
     <row r="4">
@@ -521,22 +521,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C4" t="n">
-        <v>1438.86</v>
+        <v>1323.54</v>
       </c>
       <c r="D4" t="n">
-        <v>935.89</v>
+        <v>974.6</v>
       </c>
       <c r="E4" t="n">
-        <v>87971.35000000001</v>
+        <v>87853.46000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>4361.05</v>
+        <v>4013.33</v>
       </c>
       <c r="G4" t="n">
-        <v>2763.2</v>
+        <v>2881.1</v>
       </c>
     </row>
     <row r="5">
@@ -544,22 +544,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C5" t="n">
-        <v>1423.71</v>
+        <v>1309.02</v>
       </c>
       <c r="D5" t="n">
-        <v>951.04</v>
+        <v>989.13</v>
       </c>
       <c r="E5" t="n">
-        <v>87020.31</v>
+        <v>86864.34</v>
       </c>
       <c r="F5" t="n">
-        <v>5784.76</v>
+        <v>5322.35</v>
       </c>
       <c r="G5" t="n">
-        <v>3714.24</v>
+        <v>3870.23</v>
       </c>
     </row>
     <row r="6">
@@ -567,22 +567,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C6" t="n">
-        <v>1408.32</v>
+        <v>1294.28</v>
       </c>
       <c r="D6" t="n">
-        <v>966.4299999999999</v>
+        <v>1003.86</v>
       </c>
       <c r="E6" t="n">
-        <v>86053.88</v>
+        <v>85860.47</v>
       </c>
       <c r="F6" t="n">
-        <v>7193.08</v>
+        <v>6616.63</v>
       </c>
       <c r="G6" t="n">
-        <v>4680.67</v>
+        <v>4874.09</v>
       </c>
     </row>
     <row r="7">
@@ -590,22 +590,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C7" t="n">
-        <v>1392.68</v>
+        <v>1279.32</v>
       </c>
       <c r="D7" t="n">
-        <v>982.0700000000001</v>
+        <v>1018.82</v>
       </c>
       <c r="E7" t="n">
-        <v>85071.81</v>
+        <v>84841.64999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>8585.76</v>
+        <v>7895.95</v>
       </c>
       <c r="G7" t="n">
-        <v>5662.74</v>
+        <v>5892.91</v>
       </c>
     </row>
     <row r="8">
@@ -613,22 +613,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C8" t="n">
-        <v>1376.78</v>
+        <v>1264.14</v>
       </c>
       <c r="D8" t="n">
-        <v>997.97</v>
+        <v>1034</v>
       </c>
       <c r="E8" t="n">
-        <v>84073.84</v>
+        <v>83807.64999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>9962.540000000001</v>
+        <v>9160.09</v>
       </c>
       <c r="G8" t="n">
-        <v>6660.71</v>
+        <v>6926.91</v>
       </c>
     </row>
     <row r="9">
@@ -636,22 +636,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C9" t="n">
-        <v>1360.63</v>
+        <v>1248.73</v>
       </c>
       <c r="D9" t="n">
-        <v>1014.12</v>
+        <v>1049.41</v>
       </c>
       <c r="E9" t="n">
-        <v>83059.72</v>
+        <v>82758.24000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>11323.17</v>
+        <v>10408.82</v>
       </c>
       <c r="G9" t="n">
-        <v>7674.83</v>
+        <v>7976.32</v>
       </c>
     </row>
     <row r="10">
@@ -659,22 +659,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C10" t="n">
-        <v>1344.22</v>
+        <v>1233.1</v>
       </c>
       <c r="D10" t="n">
-        <v>1030.53</v>
+        <v>1065.04</v>
       </c>
       <c r="E10" t="n">
-        <v>82029.2</v>
+        <v>81693.2</v>
       </c>
       <c r="F10" t="n">
-        <v>12667.39</v>
+        <v>11641.92</v>
       </c>
       <c r="G10" t="n">
-        <v>8705.360000000001</v>
+        <v>9041.360000000001</v>
       </c>
     </row>
     <row r="11">
@@ -682,22 +682,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C11" t="n">
-        <v>1327.54</v>
+        <v>1217.23</v>
       </c>
       <c r="D11" t="n">
-        <v>1047.21</v>
+        <v>1080.91</v>
       </c>
       <c r="E11" t="n">
-        <v>80981.99000000001</v>
+        <v>80612.28</v>
       </c>
       <c r="F11" t="n">
-        <v>13994.93</v>
+        <v>12859.15</v>
       </c>
       <c r="G11" t="n">
-        <v>9752.57</v>
+        <v>10122.27</v>
       </c>
     </row>
     <row r="12">
@@ -705,22 +705,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C12" t="n">
-        <v>1310.59</v>
+        <v>1201.12</v>
       </c>
       <c r="D12" t="n">
-        <v>1064.15</v>
+        <v>1097.02</v>
       </c>
       <c r="E12" t="n">
-        <v>79917.83</v>
+        <v>79515.25999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>15305.52</v>
+        <v>14060.27</v>
       </c>
       <c r="G12" t="n">
-        <v>10816.72</v>
+        <v>11219.29</v>
       </c>
     </row>
     <row r="13">
@@ -728,22 +728,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C13" t="n">
-        <v>1293.37</v>
+        <v>1184.78</v>
       </c>
       <c r="D13" t="n">
-        <v>1081.38</v>
+        <v>1113.36</v>
       </c>
       <c r="E13" t="n">
-        <v>78836.46000000001</v>
+        <v>78401.89999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>16598.89</v>
+        <v>15245.05</v>
       </c>
       <c r="G13" t="n">
-        <v>11898.1</v>
+        <v>12332.65</v>
       </c>
     </row>
     <row r="14">
@@ -751,22 +751,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C14" t="n">
-        <v>1275.87</v>
+        <v>1168.19</v>
       </c>
       <c r="D14" t="n">
-        <v>1098.88</v>
+        <v>1129.95</v>
       </c>
       <c r="E14" t="n">
-        <v>77737.58</v>
+        <v>77271.94</v>
       </c>
       <c r="F14" t="n">
-        <v>17874.76</v>
+        <v>16413.24</v>
       </c>
       <c r="G14" t="n">
-        <v>12996.98</v>
+        <v>13462.6</v>
       </c>
     </row>
     <row r="15">
@@ -774,22 +774,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C15" t="n">
-        <v>1258.09</v>
+        <v>1151.35</v>
       </c>
       <c r="D15" t="n">
-        <v>1116.66</v>
+        <v>1146.79</v>
       </c>
       <c r="E15" t="n">
-        <v>76620.92</v>
+        <v>76125.14999999999</v>
       </c>
       <c r="F15" t="n">
-        <v>19132.85</v>
+        <v>17564.59</v>
       </c>
       <c r="G15" t="n">
-        <v>14113.64</v>
+        <v>14609.39</v>
       </c>
     </row>
     <row r="16">
@@ -797,22 +797,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C16" t="n">
-        <v>1240.02</v>
+        <v>1134.26</v>
       </c>
       <c r="D16" t="n">
-        <v>1134.73</v>
+        <v>1163.88</v>
       </c>
       <c r="E16" t="n">
-        <v>75486.17999999999</v>
+        <v>74961.27</v>
       </c>
       <c r="F16" t="n">
-        <v>20372.87</v>
+        <v>18698.85</v>
       </c>
       <c r="G16" t="n">
-        <v>15248.37</v>
+        <v>15773.27</v>
       </c>
     </row>
     <row r="17">
@@ -820,22 +820,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C17" t="n">
-        <v>1221.65</v>
+        <v>1116.92</v>
       </c>
       <c r="D17" t="n">
-        <v>1153.1</v>
+        <v>1181.22</v>
       </c>
       <c r="E17" t="n">
-        <v>74333.08</v>
+        <v>73780.06</v>
       </c>
       <c r="F17" t="n">
-        <v>21594.52</v>
+        <v>19815.77</v>
       </c>
       <c r="G17" t="n">
-        <v>16401.47</v>
+        <v>16954.49000000001</v>
       </c>
     </row>
     <row r="18">
@@ -843,22 +843,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C18" t="n">
-        <v>1202.99</v>
+        <v>1099.32</v>
       </c>
       <c r="D18" t="n">
-        <v>1171.76</v>
+        <v>1198.82</v>
       </c>
       <c r="E18" t="n">
-        <v>73161.33</v>
+        <v>72581.24000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>22797.51</v>
+        <v>20915.09</v>
       </c>
       <c r="G18" t="n">
-        <v>17573.23</v>
+        <v>18153.31</v>
       </c>
     </row>
     <row r="19">
@@ -866,22 +866,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C19" t="n">
-        <v>1184.03</v>
+        <v>1081.46</v>
       </c>
       <c r="D19" t="n">
-        <v>1190.72</v>
+        <v>1216.68</v>
       </c>
       <c r="E19" t="n">
-        <v>71970.60000000001</v>
+        <v>71364.55</v>
       </c>
       <c r="F19" t="n">
-        <v>23981.54</v>
+        <v>21996.55</v>
       </c>
       <c r="G19" t="n">
-        <v>18763.95</v>
+        <v>19369.99000000001</v>
       </c>
     </row>
     <row r="20">
@@ -889,22 +889,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C20" t="n">
-        <v>1164.76</v>
+        <v>1063.33</v>
       </c>
       <c r="D20" t="n">
-        <v>1209.99</v>
+        <v>1234.81</v>
       </c>
       <c r="E20" t="n">
-        <v>70760.61</v>
+        <v>70129.74000000001</v>
       </c>
       <c r="F20" t="n">
-        <v>25146.3</v>
+        <v>23059.88</v>
       </c>
       <c r="G20" t="n">
-        <v>19973.94</v>
+        <v>20604.80000000001</v>
       </c>
     </row>
     <row r="21">
@@ -912,22 +912,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C21" t="n">
-        <v>1145.17</v>
+        <v>1044.93</v>
       </c>
       <c r="D21" t="n">
-        <v>1229.58</v>
+        <v>1253.21</v>
       </c>
       <c r="E21" t="n">
-        <v>69531.03</v>
+        <v>68876.53</v>
       </c>
       <c r="F21" t="n">
-        <v>26291.47</v>
+        <v>24104.81</v>
       </c>
       <c r="G21" t="n">
-        <v>21203.52</v>
+        <v>21858.01000000001</v>
       </c>
     </row>
     <row r="22">
@@ -935,22 +935,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C22" t="n">
-        <v>1125.28</v>
+        <v>1026.26</v>
       </c>
       <c r="D22" t="n">
-        <v>1249.47</v>
+        <v>1271.88</v>
       </c>
       <c r="E22" t="n">
-        <v>68281.56</v>
+        <v>67604.64999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>27416.75</v>
+        <v>25131.07</v>
       </c>
       <c r="G22" t="n">
-        <v>22452.99</v>
+        <v>23129.89000000001</v>
       </c>
     </row>
     <row r="23">
@@ -958,22 +958,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C23" t="n">
-        <v>1105.05</v>
+        <v>1007.31</v>
       </c>
       <c r="D23" t="n">
-        <v>1269.7</v>
+        <v>1290.83</v>
       </c>
       <c r="E23" t="n">
-        <v>67011.86</v>
+        <v>66313.82000000001</v>
       </c>
       <c r="F23" t="n">
-        <v>28521.8</v>
+        <v>26138.38</v>
       </c>
       <c r="G23" t="n">
-        <v>23722.69</v>
+        <v>24420.72000000001</v>
       </c>
     </row>
     <row r="24">
@@ -981,22 +981,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C24" t="n">
-        <v>1084.51</v>
+        <v>988.08</v>
       </c>
       <c r="D24" t="n">
-        <v>1290.24</v>
+        <v>1310.07</v>
       </c>
       <c r="E24" t="n">
-        <v>65721.62</v>
+        <v>65003.75</v>
       </c>
       <c r="F24" t="n">
-        <v>29606.31</v>
+        <v>27126.46</v>
       </c>
       <c r="G24" t="n">
-        <v>25012.93</v>
+        <v>25730.79000000001</v>
       </c>
     </row>
     <row r="25">
@@ -1004,22 +1004,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C25" t="n">
-        <v>1063.62</v>
+        <v>968.5599999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>1311.13</v>
+        <v>1329.59</v>
       </c>
       <c r="E25" t="n">
-        <v>64410.49</v>
+        <v>63674.17</v>
       </c>
       <c r="F25" t="n">
-        <v>30669.93</v>
+        <v>28095.02</v>
       </c>
       <c r="G25" t="n">
-        <v>26324.06</v>
+        <v>27060.38000000001</v>
       </c>
     </row>
     <row r="26">
@@ -1027,22 +1027,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C26" t="n">
-        <v>1042.41</v>
+        <v>948.75</v>
       </c>
       <c r="D26" t="n">
-        <v>1332.34</v>
+        <v>1349.4</v>
       </c>
       <c r="E26" t="n">
-        <v>63078.15</v>
+        <v>62324.77</v>
       </c>
       <c r="F26" t="n">
-        <v>31712.34</v>
+        <v>29043.77</v>
       </c>
       <c r="G26" t="n">
-        <v>27656.4</v>
+        <v>28409.78000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1050,22 +1050,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C27" t="n">
-        <v>1020.84</v>
+        <v>928.64</v>
       </c>
       <c r="D27" t="n">
-        <v>1353.91</v>
+        <v>1369.5</v>
       </c>
       <c r="E27" t="n">
-        <v>61724.24</v>
+        <v>60955.27</v>
       </c>
       <c r="F27" t="n">
-        <v>32733.18</v>
+        <v>29972.41</v>
       </c>
       <c r="G27" t="n">
-        <v>29010.31</v>
+        <v>29779.28000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1073,22 +1073,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C28" t="n">
-        <v>998.9299999999999</v>
+        <v>908.23</v>
       </c>
       <c r="D28" t="n">
-        <v>1375.82</v>
+        <v>1389.91</v>
       </c>
       <c r="E28" t="n">
-        <v>60348.42</v>
+        <v>59565.36</v>
       </c>
       <c r="F28" t="n">
-        <v>33732.10999999999</v>
+        <v>30880.64</v>
       </c>
       <c r="G28" t="n">
-        <v>30386.13</v>
+        <v>31169.19000000001</v>
       </c>
     </row>
     <row r="29">
@@ -1096,22 +1096,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C29" t="n">
-        <v>976.67</v>
+        <v>887.52</v>
       </c>
       <c r="D29" t="n">
-        <v>1398.08</v>
+        <v>1410.62</v>
       </c>
       <c r="E29" t="n">
-        <v>58950.34</v>
+        <v>58154.74</v>
       </c>
       <c r="F29" t="n">
-        <v>34708.77999999999</v>
+        <v>31768.16</v>
       </c>
       <c r="G29" t="n">
-        <v>31784.21</v>
+        <v>32579.81000000001</v>
       </c>
     </row>
     <row r="30">
@@ -1119,22 +1119,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C30" t="n">
-        <v>954.04</v>
+        <v>866.51</v>
       </c>
       <c r="D30" t="n">
-        <v>1420.71</v>
+        <v>1431.64</v>
       </c>
       <c r="E30" t="n">
-        <v>57529.63</v>
+        <v>56723.1</v>
       </c>
       <c r="F30" t="n">
-        <v>35662.81999999999</v>
+        <v>32634.67</v>
       </c>
       <c r="G30" t="n">
-        <v>33204.92</v>
+        <v>34011.45000000001</v>
       </c>
     </row>
     <row r="31">
@@ -1142,22 +1142,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C31" t="n">
-        <v>931.05</v>
+        <v>845.17</v>
       </c>
       <c r="D31" t="n">
-        <v>1443.7</v>
+        <v>1452.97</v>
       </c>
       <c r="E31" t="n">
-        <v>56085.93</v>
+        <v>55270.13</v>
       </c>
       <c r="F31" t="n">
-        <v>36593.87</v>
+        <v>33479.84</v>
       </c>
       <c r="G31" t="n">
-        <v>34648.62</v>
+        <v>35464.42000000001</v>
       </c>
     </row>
     <row r="32">
@@ -1165,22 +1165,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C32" t="n">
-        <v>907.6799999999999</v>
+        <v>823.52</v>
       </c>
       <c r="D32" t="n">
-        <v>1467.07</v>
+        <v>1474.62</v>
       </c>
       <c r="E32" t="n">
-        <v>54618.86</v>
+        <v>53795.52</v>
       </c>
       <c r="F32" t="n">
-        <v>37501.55</v>
+        <v>34303.35999999999</v>
       </c>
       <c r="G32" t="n">
-        <v>36115.69</v>
+        <v>36939.04000000002</v>
       </c>
     </row>
     <row r="33">
@@ -1188,22 +1188,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C33" t="n">
-        <v>883.9400000000001</v>
+        <v>801.55</v>
       </c>
       <c r="D33" t="n">
-        <v>1490.81</v>
+        <v>1496.59</v>
       </c>
       <c r="E33" t="n">
-        <v>53128.05</v>
+        <v>52298.93</v>
       </c>
       <c r="F33" t="n">
-        <v>38385.49</v>
+        <v>35104.91</v>
       </c>
       <c r="G33" t="n">
-        <v>37606.49999999999</v>
+        <v>38435.63000000001</v>
       </c>
     </row>
     <row r="34">
@@ -1211,22 +1211,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C34" t="n">
-        <v>859.8099999999999</v>
+        <v>779.25</v>
       </c>
       <c r="D34" t="n">
-        <v>1514.94</v>
+        <v>1518.89</v>
       </c>
       <c r="E34" t="n">
-        <v>51613.11</v>
+        <v>50780.04</v>
       </c>
       <c r="F34" t="n">
-        <v>39245.3</v>
+        <v>35884.16</v>
       </c>
       <c r="G34" t="n">
-        <v>39121.44</v>
+        <v>39954.52000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1234,22 +1234,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C35" t="n">
-        <v>835.3</v>
+        <v>756.62</v>
       </c>
       <c r="D35" t="n">
-        <v>1539.45</v>
+        <v>1541.52</v>
       </c>
       <c r="E35" t="n">
-        <v>50073.66</v>
+        <v>49238.52</v>
       </c>
       <c r="F35" t="n">
-        <v>40080.6</v>
+        <v>36640.78</v>
       </c>
       <c r="G35" t="n">
-        <v>40660.88999999999</v>
+        <v>41496.04000000001</v>
       </c>
     </row>
     <row r="36">
@@ -1257,22 +1257,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C36" t="n">
-        <v>810.38</v>
+        <v>733.65</v>
       </c>
       <c r="D36" t="n">
-        <v>1564.37</v>
+        <v>1564.49</v>
       </c>
       <c r="E36" t="n">
-        <v>48509.29</v>
+        <v>47674.03</v>
       </c>
       <c r="F36" t="n">
-        <v>40890.98</v>
+        <v>37374.43</v>
       </c>
       <c r="G36" t="n">
-        <v>42225.25999999999</v>
+        <v>43060.53000000001</v>
       </c>
     </row>
     <row r="37">
@@ -1280,22 +1280,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C37" t="n">
-        <v>785.0599999999999</v>
+        <v>710.34</v>
       </c>
       <c r="D37" t="n">
-        <v>1589.69</v>
+        <v>1587.8</v>
       </c>
       <c r="E37" t="n">
-        <v>46919.6</v>
+        <v>46086.23</v>
       </c>
       <c r="F37" t="n">
-        <v>41676.03999999999</v>
+        <v>38084.77</v>
       </c>
       <c r="G37" t="n">
-        <v>43814.95</v>
+        <v>44648.33000000001</v>
       </c>
     </row>
     <row r="38">
@@ -1303,22 +1303,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C38" t="n">
-        <v>759.34</v>
+        <v>686.6799999999999</v>
       </c>
       <c r="D38" t="n">
-        <v>1615.41</v>
+        <v>1611.46</v>
       </c>
       <c r="E38" t="n">
-        <v>45304.19</v>
+        <v>44474.77</v>
       </c>
       <c r="F38" t="n">
-        <v>42435.37999999999</v>
+        <v>38771.45</v>
       </c>
       <c r="G38" t="n">
-        <v>45430.36</v>
+        <v>46259.79000000001</v>
       </c>
     </row>
     <row r="39">
@@ -1326,22 +1326,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C39" t="n">
-        <v>733.1900000000001</v>
+        <v>662.67</v>
       </c>
       <c r="D39" t="n">
-        <v>1641.56</v>
+        <v>1635.47</v>
       </c>
       <c r="E39" t="n">
-        <v>43662.63</v>
+        <v>42839.3</v>
       </c>
       <c r="F39" t="n">
-        <v>43168.56999999999</v>
+        <v>39434.12</v>
       </c>
       <c r="G39" t="n">
-        <v>47071.92</v>
+        <v>47895.26000000001</v>
       </c>
     </row>
     <row r="40">
@@ -1349,22 +1349,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C40" t="n">
-        <v>706.63</v>
+        <v>638.3099999999999</v>
       </c>
       <c r="D40" t="n">
-        <v>1668.12</v>
+        <v>1659.84</v>
       </c>
       <c r="E40" t="n">
-        <v>41994.51</v>
+        <v>41179.47</v>
       </c>
       <c r="F40" t="n">
-        <v>43875.19999999999</v>
+        <v>40072.42999999999</v>
       </c>
       <c r="G40" t="n">
-        <v>48740.04</v>
+        <v>49555.10000000001</v>
       </c>
     </row>
     <row r="41">
@@ -1372,22 +1372,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C41" t="n">
-        <v>679.63</v>
+        <v>613.5700000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>1695.12</v>
+        <v>1684.57</v>
       </c>
       <c r="E41" t="n">
-        <v>40299.39</v>
+        <v>39494.9</v>
       </c>
       <c r="F41" t="n">
-        <v>44554.82999999999</v>
+        <v>40685.99999999999</v>
       </c>
       <c r="G41" t="n">
-        <v>50435.16</v>
+        <v>51239.67000000001</v>
       </c>
     </row>
     <row r="42">
@@ -1395,22 +1395,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C42" t="n">
-        <v>652.2</v>
+        <v>588.47</v>
       </c>
       <c r="D42" t="n">
-        <v>1722.55</v>
+        <v>1709.67</v>
       </c>
       <c r="E42" t="n">
-        <v>38576.84</v>
+        <v>37785.23</v>
       </c>
       <c r="F42" t="n">
-        <v>45207.02999999998</v>
+        <v>41274.46999999999</v>
       </c>
       <c r="G42" t="n">
-        <v>52157.71000000001</v>
+        <v>52949.34</v>
       </c>
     </row>
     <row r="43">
@@ -1418,22 +1418,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C43" t="n">
-        <v>624.3200000000001</v>
+        <v>563</v>
       </c>
       <c r="D43" t="n">
-        <v>1750.43</v>
+        <v>1735.14</v>
       </c>
       <c r="E43" t="n">
-        <v>36826.4</v>
+        <v>36050.09</v>
       </c>
       <c r="F43" t="n">
-        <v>45831.34999999998</v>
+        <v>41837.46999999999</v>
       </c>
       <c r="G43" t="n">
-        <v>53908.14000000001</v>
+        <v>54684.48</v>
       </c>
     </row>
     <row r="44">
@@ -1441,22 +1441,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C44" t="n">
-        <v>595.99</v>
+        <v>537.15</v>
       </c>
       <c r="D44" t="n">
-        <v>1778.76</v>
+        <v>1761</v>
       </c>
       <c r="E44" t="n">
-        <v>35047.65</v>
+        <v>34289.09</v>
       </c>
       <c r="F44" t="n">
-        <v>46427.33999999998</v>
+        <v>42374.62</v>
       </c>
       <c r="G44" t="n">
-        <v>55686.90000000001</v>
+        <v>56445.48</v>
       </c>
     </row>
     <row r="45">
@@ -1464,22 +1464,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C45" t="n">
-        <v>567.2</v>
+        <v>510.91</v>
       </c>
       <c r="D45" t="n">
-        <v>1807.55</v>
+        <v>1787.23</v>
       </c>
       <c r="E45" t="n">
-        <v>33240.1</v>
+        <v>32501.86</v>
       </c>
       <c r="F45" t="n">
-        <v>46994.53999999998</v>
+        <v>42885.53</v>
       </c>
       <c r="G45" t="n">
-        <v>57494.45000000001</v>
+        <v>58232.71000000001</v>
       </c>
     </row>
     <row r="46">
@@ -1487,22 +1487,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C46" t="n">
-        <v>537.95</v>
+        <v>484.28</v>
       </c>
       <c r="D46" t="n">
-        <v>1836.8</v>
+        <v>1813.86</v>
       </c>
       <c r="E46" t="n">
-        <v>31403.3</v>
+        <v>30687.99</v>
       </c>
       <c r="F46" t="n">
-        <v>47532.48999999998</v>
+        <v>43369.81</v>
       </c>
       <c r="G46" t="n">
-        <v>59331.25000000001</v>
+        <v>60046.57000000001</v>
       </c>
     </row>
     <row r="47">
@@ -1510,22 +1510,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C47" t="n">
-        <v>508.22</v>
+        <v>457.25</v>
       </c>
       <c r="D47" t="n">
-        <v>1866.53</v>
+        <v>1840.89</v>
       </c>
       <c r="E47" t="n">
-        <v>29536.77</v>
+        <v>28847.1</v>
       </c>
       <c r="F47" t="n">
-        <v>48040.70999999998</v>
+        <v>43827.06</v>
       </c>
       <c r="G47" t="n">
-        <v>61197.78000000001</v>
+        <v>61887.46000000001</v>
       </c>
     </row>
     <row r="48">
@@ -1533,22 +1533,22 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C48" t="n">
-        <v>478.02</v>
+        <v>429.82</v>
       </c>
       <c r="D48" t="n">
-        <v>1896.73</v>
+        <v>1868.32</v>
       </c>
       <c r="E48" t="n">
-        <v>27640.04</v>
+        <v>26978.78</v>
       </c>
       <c r="F48" t="n">
-        <v>48518.72999999997</v>
+        <v>44256.88</v>
       </c>
       <c r="G48" t="n">
-        <v>63094.51000000002</v>
+        <v>63755.78000000001</v>
       </c>
     </row>
     <row r="49">
@@ -1556,22 +1556,22 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C49" t="n">
-        <v>447.32</v>
+        <v>401.98</v>
       </c>
       <c r="D49" t="n">
-        <v>1927.43</v>
+        <v>1896.16</v>
       </c>
       <c r="E49" t="n">
-        <v>25712.61</v>
+        <v>25082.62</v>
       </c>
       <c r="F49" t="n">
-        <v>48966.04999999997</v>
+        <v>44658.86</v>
       </c>
       <c r="G49" t="n">
-        <v>65021.94000000002</v>
+        <v>65651.94</v>
       </c>
     </row>
     <row r="50">
@@ -1579,22 +1579,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C50" t="n">
-        <v>416.13</v>
+        <v>373.73</v>
       </c>
       <c r="D50" t="n">
-        <v>1958.62</v>
+        <v>1924.41</v>
       </c>
       <c r="E50" t="n">
-        <v>23753.99</v>
+        <v>23158.21</v>
       </c>
       <c r="F50" t="n">
-        <v>49382.17999999997</v>
+        <v>45032.59</v>
       </c>
       <c r="G50" t="n">
-        <v>66980.56000000001</v>
+        <v>67576.35000000001</v>
       </c>
     </row>
     <row r="51">
@@ -1602,22 +1602,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C51" t="n">
-        <v>384.43</v>
+        <v>345.06</v>
       </c>
       <c r="D51" t="n">
-        <v>1990.32</v>
+        <v>1953.09</v>
       </c>
       <c r="E51" t="n">
-        <v>21763.67</v>
+        <v>21205.13</v>
       </c>
       <c r="F51" t="n">
-        <v>49766.60999999997</v>
+        <v>45377.65</v>
       </c>
       <c r="G51" t="n">
-        <v>68970.88000000002</v>
+        <v>69529.44</v>
       </c>
     </row>
     <row r="52">
@@ -1625,22 +1625,22 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C52" t="n">
-        <v>352.22</v>
+        <v>315.96</v>
       </c>
       <c r="D52" t="n">
-        <v>2022.53</v>
+        <v>1982.19</v>
       </c>
       <c r="E52" t="n">
-        <v>19741.14</v>
+        <v>19222.94</v>
       </c>
       <c r="F52" t="n">
-        <v>50118.82999999997</v>
+        <v>45693.61</v>
       </c>
       <c r="G52" t="n">
-        <v>70993.41000000002</v>
+        <v>71511.63</v>
       </c>
     </row>
     <row r="53">
@@ -1648,22 +1648,22 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C53" t="n">
-        <v>319.49</v>
+        <v>286.42</v>
       </c>
       <c r="D53" t="n">
-        <v>2055.26</v>
+        <v>2011.72</v>
       </c>
       <c r="E53" t="n">
-        <v>17685.87</v>
+        <v>17211.22</v>
       </c>
       <c r="F53" t="n">
-        <v>50438.31999999997</v>
+        <v>45980.03</v>
       </c>
       <c r="G53" t="n">
-        <v>73048.67000000001</v>
+        <v>73523.35000000001</v>
       </c>
     </row>
     <row r="54">
@@ -1671,22 +1671,22 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C54" t="n">
-        <v>286.22</v>
+        <v>256.45</v>
       </c>
       <c r="D54" t="n">
-        <v>2088.53</v>
+        <v>2041.7</v>
       </c>
       <c r="E54" t="n">
-        <v>15597.35</v>
+        <v>15169.52</v>
       </c>
       <c r="F54" t="n">
-        <v>50724.53999999997</v>
+        <v>46236.48</v>
       </c>
       <c r="G54" t="n">
-        <v>75137.20000000001</v>
+        <v>75565.05</v>
       </c>
     </row>
     <row r="55">
@@ -1694,22 +1694,22 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C55" t="n">
-        <v>252.42</v>
+        <v>226.03</v>
       </c>
       <c r="D55" t="n">
-        <v>2122.33</v>
+        <v>2072.12</v>
       </c>
       <c r="E55" t="n">
-        <v>13475.02</v>
+        <v>13097.41</v>
       </c>
       <c r="F55" t="n">
-        <v>50976.95999999997</v>
+        <v>46462.50999999999</v>
       </c>
       <c r="G55" t="n">
-        <v>77259.53000000001</v>
+        <v>77637.17</v>
       </c>
     </row>
     <row r="56">
@@ -1717,22 +1717,22 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C56" t="n">
-        <v>218.08</v>
+        <v>195.15</v>
       </c>
       <c r="D56" t="n">
-        <v>2156.67</v>
+        <v>2102.99</v>
       </c>
       <c r="E56" t="n">
-        <v>11318.35</v>
+        <v>10994.42</v>
       </c>
       <c r="F56" t="n">
-        <v>51195.03999999997</v>
+        <v>46657.66</v>
       </c>
       <c r="G56" t="n">
-        <v>79416.20000000001</v>
+        <v>79740.16</v>
       </c>
     </row>
     <row r="57">
@@ -1740,22 +1740,22 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C57" t="n">
-        <v>183.17</v>
+        <v>163.82</v>
       </c>
       <c r="D57" t="n">
-        <v>2191.58</v>
+        <v>2134.33</v>
       </c>
       <c r="E57" t="n">
-        <v>9126.77</v>
+        <v>8860.09</v>
       </c>
       <c r="F57" t="n">
-        <v>51378.20999999997</v>
+        <v>46821.48</v>
       </c>
       <c r="G57" t="n">
-        <v>81607.78000000001</v>
+        <v>81874.49000000001</v>
       </c>
     </row>
     <row r="58">
@@ -1763,22 +1763,22 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C58" t="n">
-        <v>147.71</v>
+        <v>132.02</v>
       </c>
       <c r="D58" t="n">
-        <v>2227.04</v>
+        <v>2166.13</v>
       </c>
       <c r="E58" t="n">
-        <v>6899.73</v>
+        <v>6693.96</v>
       </c>
       <c r="F58" t="n">
-        <v>51525.91999999997</v>
+        <v>46953.49999999999</v>
       </c>
       <c r="G58" t="n">
-        <v>83834.82000000001</v>
+        <v>84040.62000000001</v>
       </c>
     </row>
     <row r="59">
@@ -1786,22 +1786,22 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C59" t="n">
-        <v>111.66</v>
+        <v>99.73999999999999</v>
       </c>
       <c r="D59" t="n">
-        <v>2263.09</v>
+        <v>2198.4</v>
       </c>
       <c r="E59" t="n">
-        <v>4636.64</v>
+        <v>4495.56</v>
       </c>
       <c r="F59" t="n">
-        <v>51637.57999999997</v>
+        <v>47053.23999999999</v>
       </c>
       <c r="G59" t="n">
-        <v>86097.91</v>
+        <v>86239.02</v>
       </c>
     </row>
     <row r="60">
@@ -1809,22 +1809,22 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C60" t="n">
-        <v>75.04000000000001</v>
+        <v>66.98</v>
       </c>
       <c r="D60" t="n">
-        <v>2299.71</v>
+        <v>2231.16</v>
       </c>
       <c r="E60" t="n">
-        <v>2336.93</v>
+        <v>2264.4</v>
       </c>
       <c r="F60" t="n">
-        <v>51712.61999999997</v>
+        <v>47120.21999999999</v>
       </c>
       <c r="G60" t="n">
-        <v>88397.62000000001</v>
+        <v>88470.18000000001</v>
       </c>
     </row>
     <row r="61">
@@ -1832,22 +1832,22 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>2374.75</v>
+        <v>2298.14</v>
       </c>
       <c r="C61" t="n">
-        <v>37.82</v>
+        <v>33.74</v>
       </c>
       <c r="D61" t="n">
-        <v>2336.93</v>
+        <v>2264.4</v>
       </c>
       <c r="E61" t="n">
         <v>-0</v>
       </c>
       <c r="F61" t="n">
-        <v>51750.43999999997</v>
+        <v>47153.95999999999</v>
       </c>
       <c r="G61" t="n">
-        <v>90734.55</v>
+        <v>90734.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>